<commit_message>
Simplex method for Swedish steel
</commit_message>
<xml_diff>
--- a/Python/Simplex_polyhedron.xlsx
+++ b/Python/Simplex_polyhedron.xlsx
@@ -34,10 +34,10 @@
     <t>[0]</t>
   </si>
   <si>
-    <t>[0. 0. 3.]</t>
-  </si>
-  <si>
-    <t>[3. 0. 0.]</t>
+    <t>[0. 0. 1.]</t>
+  </si>
+  <si>
+    <t>[1. 0. 0.]</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>